<commit_message>
Separated total sums for outputs and transport exchanges with shoots for main model's pools and processes properties. Added cytokinins production and balance whose export is then computed by the shoot model
</commit_message>
<xml_diff>
--- a/doc/Propriétés_RhizoDep.xlsx
+++ b/doc/Propriétés_RhizoDep.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0BEA97-17BC-46C6-B6C1-B5DC33ECD68F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103DFF63-BA63-4226-936F-EC4AB352652E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -625,7 +625,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,8 +916,8 @@
   <dimension ref="A1:D127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,7 +985,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5">
@@ -998,7 +997,7 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1010,7 +1009,7 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5">
@@ -1022,7 +1021,7 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5">
@@ -1034,7 +1033,7 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5">
@@ -1074,7 +1073,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="5">
@@ -1086,7 +1085,7 @@
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="5">
@@ -1098,7 +1097,7 @@
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="5">
@@ -1110,7 +1109,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="6">
@@ -1122,7 +1121,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="5">
@@ -1134,7 +1133,7 @@
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="5">
@@ -1146,7 +1145,7 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="5">
@@ -1158,7 +1157,7 @@
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="5">
@@ -1170,7 +1169,7 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="5">
@@ -1182,7 +1181,7 @@
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="5">
@@ -1194,7 +1193,7 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="5">
@@ -1206,7 +1205,7 @@
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="5">
@@ -1218,7 +1217,7 @@
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="5">
@@ -1230,7 +1229,7 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1242,7 +1241,7 @@
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="5">
@@ -1254,7 +1253,7 @@
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="5">
@@ -1266,7 +1265,7 @@
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="5">
@@ -1292,7 +1291,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="5">
@@ -1304,7 +1303,7 @@
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="5">
@@ -1316,7 +1315,7 @@
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="5">
@@ -1396,7 +1395,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B38" s="5">
@@ -1408,7 +1407,7 @@
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="5">
@@ -1420,7 +1419,7 @@
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="5">
@@ -1432,7 +1431,7 @@
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="5">
@@ -1456,7 +1455,7 @@
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="5">
@@ -1468,7 +1467,7 @@
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B44" s="5">
@@ -1522,7 +1521,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="5">
@@ -1534,7 +1533,7 @@
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B49" s="5">
@@ -1546,7 +1545,7 @@
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="5">
@@ -1558,7 +1557,7 @@
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B51" s="5">
@@ -1570,7 +1569,7 @@
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B52" s="5">
@@ -1582,7 +1581,7 @@
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B53" s="5">
@@ -1594,7 +1593,7 @@
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B54" s="5">
@@ -1606,7 +1605,7 @@
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="5">
@@ -1646,7 +1645,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B58" s="5">
@@ -1658,7 +1657,7 @@
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B59" s="5">
@@ -1740,7 +1739,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B65" s="5">
@@ -1752,7 +1751,7 @@
       <c r="D65" s="1"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B66" s="5">
@@ -1764,7 +1763,7 @@
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B67" s="5">
@@ -1776,7 +1775,7 @@
       <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B68" s="5">
@@ -1788,7 +1787,7 @@
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B69" s="5">
@@ -1800,7 +1799,7 @@
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B70" s="5">
@@ -1812,7 +1811,7 @@
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B71" s="5">
@@ -1824,7 +1823,7 @@
       <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B72" s="5">
@@ -1836,7 +1835,7 @@
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B73" s="5">
@@ -1848,7 +1847,7 @@
       <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B74" s="5">
@@ -1860,7 +1859,7 @@
       <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B75" s="5">
@@ -1872,7 +1871,7 @@
       <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B76" s="5">
@@ -1884,7 +1883,7 @@
       <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B77" s="5">
@@ -1896,7 +1895,7 @@
       <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B78" s="5">
@@ -1908,7 +1907,7 @@
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B79" s="5">
@@ -1920,7 +1919,7 @@
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B80" s="5">
@@ -1932,7 +1931,7 @@
       <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B81" s="5">
@@ -1944,7 +1943,7 @@
       <c r="D81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B82" s="5">
@@ -1956,7 +1955,7 @@
       <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B83" s="5">
@@ -1968,7 +1967,7 @@
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B84" s="5">
@@ -1980,7 +1979,7 @@
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B85" s="5">
@@ -1992,7 +1991,7 @@
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B86" s="5">
@@ -2004,7 +2003,7 @@
       <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="8" t="s">
+      <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B87" s="5">
@@ -2016,7 +2015,7 @@
       <c r="D87" s="1"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B88" s="5">
@@ -2028,7 +2027,7 @@
       <c r="D88" s="1"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="8" t="s">
+      <c r="A89" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B89" s="5">
@@ -2040,7 +2039,7 @@
       <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B90" s="5">
@@ -2052,7 +2051,7 @@
       <c r="D90" s="1"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="8" t="s">
+      <c r="A91" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B91" s="5">
@@ -2064,7 +2063,7 @@
       <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="8" t="s">
+      <c r="A92" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B92" s="5">
@@ -2076,7 +2075,7 @@
       <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="8" t="s">
+      <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B93" s="5">
@@ -2088,7 +2087,7 @@
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B94" s="5">
@@ -2100,7 +2099,7 @@
       <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B95" s="5" t="s">
@@ -2112,7 +2111,7 @@
       <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B96" s="5">
@@ -2124,7 +2123,7 @@
       <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="8" t="s">
+      <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B97" s="5">
@@ -2136,7 +2135,7 @@
       <c r="D97" s="1"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="8" t="s">
+      <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B98" s="5">
@@ -2148,7 +2147,7 @@
       <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="8" t="s">
+      <c r="A99" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B99" s="5">
@@ -2160,7 +2159,7 @@
       <c r="D99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="8" t="s">
+      <c r="A100" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B100" s="5">
@@ -2172,7 +2171,7 @@
       <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="8" t="s">
+      <c r="A101" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B101" s="5">
@@ -2184,7 +2183,7 @@
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="8" t="s">
+      <c r="A102" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B102" s="5">
@@ -2196,7 +2195,7 @@
       <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="8" t="s">
+      <c r="A103" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B103" s="5">
@@ -2208,7 +2207,7 @@
       <c r="D103" s="1"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B104" s="5">
@@ -2220,7 +2219,7 @@
       <c r="D104" s="1"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="8" t="s">
+      <c r="A105" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B105" s="5">
@@ -2232,7 +2231,7 @@
       <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="8" t="s">
+      <c r="A106" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B106" s="5">
@@ -2244,7 +2243,7 @@
       <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="8" t="s">
+      <c r="A107" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B107" s="5">
@@ -2256,7 +2255,7 @@
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="8" t="s">
+      <c r="A108" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B108" s="5">
@@ -2268,7 +2267,7 @@
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="8" t="s">
+      <c r="A109" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B109" s="5" t="s">
@@ -2280,7 +2279,7 @@
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="8" t="s">
+      <c r="A110" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B110" s="5" t="s">
@@ -2292,7 +2291,7 @@
       <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="8" t="s">
+      <c r="A111" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B111" s="5" t="s">
@@ -2304,7 +2303,7 @@
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="8" t="s">
+      <c r="A112" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B112" s="5">
@@ -2316,7 +2315,7 @@
       <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="8" t="s">
+      <c r="A113" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B113" s="5">
@@ -2328,7 +2327,7 @@
       <c r="D113" s="1"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="8" t="s">
+      <c r="A114" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B114" s="5">
@@ -2340,7 +2339,7 @@
       <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="8" t="s">
+      <c r="A115" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B115" s="5">
@@ -2352,7 +2351,7 @@
       <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="8" t="s">
+      <c r="A116" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B116" s="5">
@@ -2364,7 +2363,7 @@
       <c r="D116" s="1"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="8" t="s">
+      <c r="A117" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B117" s="5">
@@ -2376,7 +2375,7 @@
       <c r="D117" s="1"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="8" t="s">
+      <c r="A118" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B118" s="5">
@@ -2388,7 +2387,7 @@
       <c r="D118" s="1"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B119" s="5">
@@ -2400,7 +2399,7 @@
       <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="8" t="s">
+      <c r="A120" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B120" s="5">
@@ -2412,7 +2411,7 @@
       <c r="D120" s="1"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="8" t="s">
+      <c r="A121" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B121" s="5">
@@ -2424,7 +2423,7 @@
       <c r="D121" s="1"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="8" t="s">
+      <c r="A122" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B122" s="5">
@@ -2436,7 +2435,7 @@
       <c r="D122" s="1"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="8" t="s">
+      <c r="A123" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B123" s="5">
@@ -2448,7 +2447,7 @@
       <c r="D123" s="1"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="8" t="s">
+      <c r="A124" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B124" s="5">
@@ -2460,7 +2459,7 @@
       <c r="D124" s="1"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="8" t="s">
+      <c r="A125" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B125" s="5">
@@ -2472,7 +2471,7 @@
       <c r="D125" s="1"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="8" t="s">
+      <c r="A126" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B126" s="5">
@@ -2484,7 +2483,7 @@
       <c r="D126" s="1"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="8" t="s">
+      <c r="A127" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B127" s="5">

</xml_diff>

<commit_message>
inserted as FSPM output
</commit_message>
<xml_diff>
--- a/doc/Propriétés_RhizoDep.xlsx
+++ b/doc/Propriétés_RhizoDep.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103DFF63-BA63-4226-936F-EC4AB352652E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{818276F8-6CE3-4C63-8F63-7CA23259AEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -571,12 +572,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -606,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -625,6 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,15 +924,15 @@
   <dimension ref="A1:D127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46:C46"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.5546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
     <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1381,7 +1389,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="5">

</xml_diff>